<commit_message>
Complete charts for MLP results
</commit_message>
<xml_diff>
--- a/Software Project 1/Source/results/mlp_fashionmnist.xlsx
+++ b/Software Project 1/Source/results/mlp_fashionmnist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan\GitHub\MachineLearning\Software Project 1\Source\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A1CDBC-A5CB-4D8A-8AAF-9CA65DFEA2D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E178B28-EC92-48D7-813B-DDB1F611D495}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -673,321 +673,6 @@
             </a:br>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Test Loss</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ro-RO"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>mlp_fashionmnist!$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>test_loss</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>mlp_fashionmnist!$H$2:$H$4</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1HL 800</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2HL 250-100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3HL 300-125-50</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>mlp_fashionmnist!$I$2:$I$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.39653808772563898</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.40992932915687502</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.40395419001579203</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EE14-4A32-B91D-6E89102C98E8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="64155568"/>
-        <c:axId val="55709392"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="64155568"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ro-RO"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="55709392"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="55709392"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ro-RO"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="64155568"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="ro-RO"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>MLP (FashionMNIST)</a:t>
-            </a:r>
-            <a:br>
-              <a:rPr lang="en-US"/>
-            </a:br>
-            <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>Test Accuracy</a:t>
             </a:r>
           </a:p>
@@ -1259,7 +944,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1296,7 +981,7 @@
               <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>MLP (FashionMNIST)</a:t>
+              <a:t>MLP</a:t>
             </a:r>
             <a:br>
               <a:rPr lang="en-US"/>
@@ -1575,7 +1260,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2310,46 +1995,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3357,7 +3002,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3465,6 +3110,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -3475,6 +3125,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -3506,519 +3161,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
@@ -4379,8 +3521,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>640080</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1451170</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
@@ -4388,7 +3530,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>22860</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -4403,33 +3545,12 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5593080" y="1356360"/>
-          <a:ext cx="13975080" cy="2750820"/>
-          <a:chOff x="5928360" y="1272540"/>
-          <a:chExt cx="10820400" cy="2750820"/>
+          <a:off x="10435150" y="1356360"/>
+          <a:ext cx="9133010" cy="2743200"/>
+          <a:chOff x="9677400" y="1272540"/>
+          <a:chExt cx="7071360" cy="2743200"/>
         </a:xfrm>
       </xdr:grpSpPr>
-      <xdr:graphicFrame macro="">
-        <xdr:nvGraphicFramePr>
-          <xdr:cNvPr id="4" name="Chart 3">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A682F99B-55FC-4206-8F01-495390C479A8}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvGraphicFramePr/>
-        </xdr:nvGraphicFramePr>
-        <xdr:xfrm>
-          <a:off x="5928360" y="1280160"/>
-          <a:ext cx="3261360" cy="2743200"/>
-        </xdr:xfrm>
-        <a:graphic>
-          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          </a:graphicData>
-        </a:graphic>
-      </xdr:graphicFrame>
       <xdr:graphicFrame macro="">
         <xdr:nvGraphicFramePr>
           <xdr:cNvPr id="5" name="Chart 4">
@@ -4447,7 +3568,7 @@
         </xdr:xfrm>
         <a:graphic>
           <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           </a:graphicData>
         </a:graphic>
       </xdr:graphicFrame>
@@ -4468,7 +3589,7 @@
         </xdr:xfrm>
         <a:graphic>
           <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           </a:graphicData>
         </a:graphic>
       </xdr:graphicFrame>
@@ -4505,7 +3626,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4813,8 +3934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M53" sqref="M53"/>
+    <sheetView tabSelected="1" topLeftCell="E31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>